<commit_message>
finally imported cswiftv to start parsing in csv files
</commit_message>
<xml_diff>
--- a/Wild-Medicine/Project Data.xlsx
+++ b/Wild-Medicine/Project Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ethanberman/Documents/comp4/Wild-Medicine/Wild-Medicine/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83FDD83F-DB4B-6E42-8075-53241C5786F8}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5CDA070F-582D-5D48-9F7B-00453BFEC29D}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2760" yWindow="1560" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{0C642D5E-428E-364E-A24F-05913C2CD676}"/>
   </bookViews>
@@ -18,6 +18,7 @@
     <sheet name="Lookup" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="116">
   <si>
     <t>Mechanism of Injury</t>
   </si>
@@ -285,6 +286,96 @@
   </si>
   <si>
     <t>HAPE</t>
+  </si>
+  <si>
+    <t>Rapid Evac</t>
+  </si>
+  <si>
+    <t>Myocardial Infarcation</t>
+  </si>
+  <si>
+    <t>Evac all patients with suspected cardiac chset pain, rapid evac any patient with a new onset of chest pain that is not clearly musculoskeletal</t>
+  </si>
+  <si>
+    <t>Reduce anxiety and activity, Place patient in position of comfort, support patient with personal medications</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lightheadedness, dizziness, anxiety, denial, radiating pain, persistent chest pain, </t>
+  </si>
+  <si>
+    <t>Hyperventilation</t>
+  </si>
+  <si>
+    <t>Pulmonary Emboism</t>
+  </si>
+  <si>
+    <t>Pnuemonia</t>
+  </si>
+  <si>
+    <t>productive cough, wet lung sounds, malaise, fatigue, shortness of breath</t>
+  </si>
+  <si>
+    <t>Asthma</t>
+  </si>
+  <si>
+    <t>Stroke</t>
+  </si>
+  <si>
+    <t>Seizure</t>
+  </si>
+  <si>
+    <t>Syncope</t>
+  </si>
+  <si>
+    <t>Gastroenteritis</t>
+  </si>
+  <si>
+    <t>Mild/Moderate Allergic Reactions</t>
+  </si>
+  <si>
+    <t>Anaphylaxis</t>
+  </si>
+  <si>
+    <t>Hyperglycemia</t>
+  </si>
+  <si>
+    <t>Hypoglycemia</t>
+  </si>
+  <si>
+    <t>Painful Menstruation</t>
+  </si>
+  <si>
+    <t>Ectopic Pregnancy</t>
+  </si>
+  <si>
+    <t>Vaginitis</t>
+  </si>
+  <si>
+    <t>UTI</t>
+  </si>
+  <si>
+    <t>Testicular Torsion</t>
+  </si>
+  <si>
+    <t>Epididymitis</t>
+  </si>
+  <si>
+    <t>Inguinal Hernia</t>
+  </si>
+  <si>
+    <t>Stress Injury</t>
+  </si>
+  <si>
+    <t>Anxiety</t>
+  </si>
+  <si>
+    <t>Depression</t>
+  </si>
+  <si>
+    <t>Mania/Psychosis</t>
+  </si>
+  <si>
+    <t>Suicidal Thoughts</t>
   </si>
 </sst>
 </file>
@@ -1049,10 +1140,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7419614-C196-954C-80FF-0975478890DC}">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1187,29 +1278,172 @@
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="K20" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>85</v>
+      </c>
+      <c r="K21" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>87</v>
+      </c>
+      <c r="I22" t="s">
+        <v>90</v>
+      </c>
+      <c r="J22" t="s">
+        <v>89</v>
+      </c>
+      <c r="K22" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>93</v>
+      </c>
+      <c r="I25" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
work on ailment and table lookup
</commit_message>
<xml_diff>
--- a/Wild-Medicine/Project Data.xlsx
+++ b/Wild-Medicine/Project Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ethanberman/Documents/comp4/Wild-Medicine/Wild-Medicine/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5CDA070F-582D-5D48-9F7B-00453BFEC29D}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F1DCD6F-C443-EE4D-A883-DA2CF20BEC9F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2760" yWindow="1560" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{0C642D5E-428E-364E-A24F-05913C2CD676}"/>
   </bookViews>
@@ -18,7 +18,6 @@
     <sheet name="Lookup" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="125">
   <si>
     <t>Mechanism of Injury</t>
   </si>
@@ -189,9 +188,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Symptom Keywords</t>
-  </si>
-  <si>
     <t>Treatments</t>
   </si>
   <si>
@@ -204,9 +200,6 @@
     <t>Treat the Cause, Calm patient, Maintain normal temperature</t>
   </si>
   <si>
-    <t>anxious, restless, disoriented, nausea, vomiting, dizziness</t>
-  </si>
-  <si>
     <t>Evac</t>
   </si>
   <si>
@@ -376,6 +369,39 @@
   </si>
   <si>
     <t>Suicidal Thoughts</t>
+  </si>
+  <si>
+    <t>anxious, restless, disoriented</t>
+  </si>
+  <si>
+    <t>worsening, eventually unresponsive</t>
+  </si>
+  <si>
+    <t>Rapid, weak, eventually slows</t>
+  </si>
+  <si>
+    <t>pale, cool, clammy</t>
+  </si>
+  <si>
+    <t>Continues to increase, becomes shallower</t>
+  </si>
+  <si>
+    <t>Falls, radial pulse weakens</t>
+  </si>
+  <si>
+    <t>Slower to respond</t>
+  </si>
+  <si>
+    <t>rapid, weak, eventually slows</t>
+  </si>
+  <si>
+    <t>rapid and shallow</t>
+  </si>
+  <si>
+    <t>pale, cool, and clammy</t>
+  </si>
+  <si>
+    <t>nausea, vomiting, dizziness</t>
   </si>
 </sst>
 </file>
@@ -1142,15 +1168,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7419614-C196-954C-80FF-0975478890DC}">
   <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.83203125" customWidth="1"/>
-    <col min="2" max="2" width="23.5" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" customWidth="1"/>
+    <col min="2" max="2" width="30.1640625" customWidth="1"/>
+    <col min="3" max="3" width="24.5" customWidth="1"/>
+    <col min="4" max="4" width="17.1640625" customWidth="1"/>
     <col min="9" max="9" width="21.1640625" customWidth="1"/>
     <col min="10" max="10" width="22.1640625" customWidth="1"/>
     <col min="11" max="11" width="15" customWidth="1"/>
@@ -1161,289 +1188,319 @@
         <v>52</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>67</v>
-      </c>
       <c r="I1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="J1" s="3" t="s">
-        <v>54</v>
-      </c>
       <c r="K1" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>54</v>
+      </c>
+      <c r="B2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F2" t="s">
+        <v>119</v>
+      </c>
+      <c r="G2" t="s">
+        <v>120</v>
       </c>
       <c r="I2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D3" t="s">
+        <v>122</v>
+      </c>
+      <c r="E3" t="s">
+        <v>123</v>
+      </c>
+      <c r="I3" t="s">
+        <v>124</v>
+      </c>
+      <c r="J3" t="s">
         <v>56</v>
-      </c>
-      <c r="I3" t="s">
-        <v>58</v>
-      </c>
-      <c r="J3" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>82</v>
+      </c>
+      <c r="K20" t="s">
         <v>84</v>
-      </c>
-      <c r="K20" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="K21" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>85</v>
+      </c>
+      <c r="I22" t="s">
+        <v>88</v>
+      </c>
+      <c r="J22" t="s">
         <v>87</v>
       </c>
-      <c r="I22" t="s">
-        <v>90</v>
-      </c>
-      <c r="J22" t="s">
-        <v>89</v>
-      </c>
       <c r="K22" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I25" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>